<commit_message>
Refactor code and remove unnecessary files
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\URA\URA-word-seperator\bahnar-word-split-and-example-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81467521-5D85-4A2B-B5F7-B61169D5A9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D1BF9A-C0A9-445D-8D48-43430FF9047E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>A</t>
   </si>
@@ -34,16 +34,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>hai</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>một</t>
-  </si>
-  <si>
-    <t>one</t>
+    <t>một nửa</t>
+  </si>
+  <si>
+    <t>a half</t>
   </si>
 </sst>
 </file>
@@ -67,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -102,11 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,24 +432,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>